<commit_message>
Landing page of Creating new project
</commit_message>
<xml_diff>
--- a/ComponentsInFields.xlsx
+++ b/ComponentsInFields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Mobiwise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0482B36-B82B-485C-A893-0EE433378442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0302AD14-41BB-488F-A214-7196C25F51F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA9AF105-AA01-4144-8C07-A98DD008D4DB}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>Save</t>
   </si>
   <si>
-    <t xml:space="preserve">Separator </t>
-  </si>
-  <si>
     <t>Geotag</t>
   </si>
   <si>
@@ -94,19 +91,29 @@
   </si>
   <si>
     <t>Data List</t>
+  </si>
+  <si>
+    <t>Separator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,8 +136,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +458,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,17 +533,17 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -541,7 +551,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes after running Adding Printer script
</commit_message>
<xml_diff>
--- a/ComponentsInFields.xlsx
+++ b/ComponentsInFields.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Mobiwise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0302AD14-41BB-488F-A214-7196C25F51F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80776050-6F50-402E-9E27-D0476B15BC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA9AF105-AA01-4144-8C07-A98DD008D4DB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Navigation</t>
   </si>
@@ -94,13 +94,16 @@
   </si>
   <si>
     <t>Separator</t>
+  </si>
+  <si>
+    <t>Printer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +117,13 @@
       <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF297BDE"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,9 +146,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -458,10 +471,10 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
@@ -475,7 +488,7 @@
     <col min="11" max="12" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -521,7 +534,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -529,7 +542,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -545,8 +558,11 @@
       <c r="E4" t="s">
         <v>20</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -556,5 +572,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>